<commit_message>
Classified La Porta (1996) and Lakonishok, Shleifer, and Vishny (1994) as Value and Fundamental growth (before it was only value, which seems misleading)
</commit_message>
<xml_diff>
--- a/Paper/new_classification.xlsx
+++ b/Paper/new_classification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tij2\Dropbox\Research\Active projects\Factors and Citations\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F25651-0608-4AB6-A220-DD3FC386B909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371AB915-1302-4D32-95D1-B0BFDD87D96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="16560" xr2:uid="{E36FB928-19B6-4E8D-A509-13CE53557E10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="61656" windowHeight="16776" xr2:uid="{E36FB928-19B6-4E8D-A509-13CE53557E10}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="783">
   <si>
     <t>name_new</t>
   </si>
@@ -2552,9 +2552,6 @@
     <t>Paper is mostly about the value factor, but indepedently proposes the equity issuance factor. I'm not sure how to classify the intangible return part. It strikes me as a momentum factor, but that seems wrong whjen it's positively related to value</t>
   </si>
   <si>
-    <t>It seems like the paper is mostly about explaining value</t>
-  </si>
-  <si>
     <t>Earnings increases</t>
   </si>
   <si>
@@ -2709,6 +2706,12 @@
   </si>
   <si>
     <t>Equity issuance/debt issuance/firm issuance</t>
+  </si>
+  <si>
+    <t>Value/Fundamental growth</t>
+  </si>
+  <si>
+    <t>It seems like the paper is mostly about explaining value, but is the first to introduce the concept of fundamental growth</t>
   </si>
 </sst>
 </file>
@@ -3176,9 +3179,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2037E566-7673-4AC3-8F27-C34FCECE148A}">
   <dimension ref="A1:M256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3284,7 +3287,7 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="14" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="G3" t="s">
         <v>691</v>
@@ -3293,10 +3296,10 @@
         <v>691</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="J3" t="s">
         <v>776</v>
-      </c>
-      <c r="J3" t="s">
-        <v>777</v>
       </c>
       <c r="K3" s="11">
         <v>0</v>
@@ -3305,7 +3308,7 @@
         <v>686</v>
       </c>
       <c r="M3" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -3653,7 +3656,7 @@
         <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>689</v>
+        <v>781</v>
       </c>
       <c r="H13" t="s">
         <v>689</v>
@@ -3694,10 +3697,10 @@
         <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>689</v>
+        <v>781</v>
       </c>
       <c r="H14" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>52</v>
@@ -3732,10 +3735,10 @@
         <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>689</v>
+        <v>781</v>
       </c>
       <c r="H15" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>52</v>
@@ -5786,10 +5789,10 @@
         <v>218</v>
       </c>
       <c r="G72" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H72" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>219</v>
@@ -6025,10 +6028,10 @@
         <v>238</v>
       </c>
       <c r="G79" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H79" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>117</v>
@@ -6099,7 +6102,7 @@
         <v>247</v>
       </c>
       <c r="G81" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H81" t="s">
         <v>694</v>
@@ -6134,7 +6137,7 @@
         <v>247</v>
       </c>
       <c r="G82" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H82" t="s">
         <v>694</v>
@@ -6442,10 +6445,10 @@
         <v>275</v>
       </c>
       <c r="G91" t="s">
-        <v>689</v>
+        <v>781</v>
       </c>
       <c r="H91" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I91" s="5" t="s">
         <v>117</v>
@@ -6457,7 +6460,7 @@
         <v>686</v>
       </c>
       <c r="M91" t="s">
-        <v>729</v>
+        <v>782</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6480,10 +6483,10 @@
         <v>279</v>
       </c>
       <c r="G92" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="H92" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I92" s="5" t="s">
         <v>219</v>
@@ -6495,7 +6498,7 @@
         <v>686</v>
       </c>
       <c r="M92" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6533,7 +6536,7 @@
         <v>686</v>
       </c>
       <c r="M93" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6571,7 +6574,7 @@
         <v>686</v>
       </c>
       <c r="M94" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6627,10 +6630,10 @@
         <v>293</v>
       </c>
       <c r="G96" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H96" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I96" s="5" t="s">
         <v>151</v>
@@ -6642,7 +6645,7 @@
         <v>686</v>
       </c>
       <c r="M96" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6663,10 +6666,10 @@
         <v>293</v>
       </c>
       <c r="G97" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H97" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I97" s="5" t="s">
         <v>151</v>
@@ -6693,10 +6696,10 @@
         <v>293</v>
       </c>
       <c r="G98" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H98" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I98" s="5" t="s">
         <v>151</v>
@@ -6723,10 +6726,10 @@
         <v>298</v>
       </c>
       <c r="G99" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H99" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I99" s="5" t="s">
         <v>52</v>
@@ -6753,10 +6756,10 @@
         <v>298</v>
       </c>
       <c r="G100" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H100" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I100" s="5" t="s">
         <v>52</v>
@@ -6783,10 +6786,10 @@
         <v>298</v>
       </c>
       <c r="G101" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H101" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I101" s="5" t="s">
         <v>52</v>
@@ -6827,7 +6830,7 @@
         <v>305</v>
       </c>
       <c r="M102" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6863,7 +6866,7 @@
         <v>686</v>
       </c>
       <c r="M103" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6886,7 +6889,7 @@
         <v>313</v>
       </c>
       <c r="G104" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H104" t="s">
         <v>681</v>
@@ -6918,7 +6921,7 @@
         <v>313</v>
       </c>
       <c r="G105" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H105" t="s">
         <v>704</v>
@@ -6933,7 +6936,7 @@
         <v>686</v>
       </c>
       <c r="M105" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -6986,10 +6989,10 @@
         <v>322</v>
       </c>
       <c r="G107" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H107" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I107" s="5" t="s">
         <v>243</v>
@@ -7018,10 +7021,10 @@
         <v>322</v>
       </c>
       <c r="G108" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H108" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I108" s="5" t="s">
         <v>243</v>
@@ -7050,10 +7053,10 @@
         <v>322</v>
       </c>
       <c r="G109" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H109" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I109" s="5" t="s">
         <v>243</v>
@@ -7082,10 +7085,10 @@
         <v>322</v>
       </c>
       <c r="G110" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H110" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I110" s="5" t="s">
         <v>243</v>
@@ -7114,10 +7117,10 @@
         <v>322</v>
       </c>
       <c r="G111" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H111" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I111" s="5" t="s">
         <v>243</v>
@@ -7144,10 +7147,10 @@
         <v>322</v>
       </c>
       <c r="G112" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H112" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I112" s="5" t="s">
         <v>243</v>
@@ -7176,10 +7179,10 @@
         <v>322</v>
       </c>
       <c r="G113" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H113" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I113" s="5" t="s">
         <v>243</v>
@@ -7206,10 +7209,10 @@
         <v>336</v>
       </c>
       <c r="G114" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="H114" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I114" s="5" t="s">
         <v>43</v>
@@ -7236,10 +7239,10 @@
         <v>336</v>
       </c>
       <c r="G115" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="H115" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I115" s="5" t="s">
         <v>43</v>
@@ -7266,10 +7269,10 @@
         <v>340</v>
       </c>
       <c r="G116" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H116" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I116" s="5" t="s">
         <v>117</v>
@@ -7296,10 +7299,10 @@
         <v>340</v>
       </c>
       <c r="G117" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H117" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I117" s="5" t="s">
         <v>117</v>
@@ -7328,10 +7331,10 @@
         <v>345</v>
       </c>
       <c r="G118" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H118" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="I118" s="5" t="s">
         <v>346</v>
@@ -7343,7 +7346,7 @@
         <v>686</v>
       </c>
       <c r="M118" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="119" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -7366,7 +7369,7 @@
         <v>345</v>
       </c>
       <c r="G119" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H119" t="s">
         <v>694</v>
@@ -7398,10 +7401,10 @@
         <v>345</v>
       </c>
       <c r="G120" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H120" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I120" s="5" t="s">
         <v>346</v>
@@ -7430,7 +7433,7 @@
         <v>345</v>
       </c>
       <c r="G121" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H121" t="s">
         <v>700</v>
@@ -7445,7 +7448,7 @@
         <v>686</v>
       </c>
       <c r="M121" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="122" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -7466,10 +7469,10 @@
         <v>355</v>
       </c>
       <c r="G122" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H122" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I122" s="5" t="s">
         <v>117</v>
@@ -7498,10 +7501,10 @@
         <v>359</v>
       </c>
       <c r="G123" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H123" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I123" s="5" t="s">
         <v>113</v>
@@ -7530,10 +7533,10 @@
         <v>359</v>
       </c>
       <c r="G124" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H124" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I124" s="5" t="s">
         <v>113</v>
@@ -7592,10 +7595,10 @@
         <v>368</v>
       </c>
       <c r="G126" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H126" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="I126" s="5" t="s">
         <v>213</v>
@@ -7607,7 +7610,7 @@
         <v>686</v>
       </c>
       <c r="M126" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="127" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -7628,7 +7631,7 @@
         <v>372</v>
       </c>
       <c r="G127" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="H127" t="s">
         <v>681</v>
@@ -7692,7 +7695,7 @@
         <v>380</v>
       </c>
       <c r="G129" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H129" t="s">
         <v>694</v>
@@ -7724,7 +7727,7 @@
         <v>380</v>
       </c>
       <c r="G130" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H130" t="s">
         <v>694</v>
@@ -7756,7 +7759,7 @@
         <v>380</v>
       </c>
       <c r="G131" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H131" t="s">
         <v>694</v>
@@ -7788,10 +7791,10 @@
         <v>388</v>
       </c>
       <c r="G132" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H132" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I132" s="5" t="s">
         <v>178</v>
@@ -7820,7 +7823,7 @@
         <v>388</v>
       </c>
       <c r="G133" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H133" t="s">
         <v>726</v>
@@ -7852,10 +7855,10 @@
         <v>388</v>
       </c>
       <c r="G134" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H134" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I134" s="5" t="s">
         <v>178</v>
@@ -7896,7 +7899,7 @@
         <v>397</v>
       </c>
       <c r="M135" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="136" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -7963,7 +7966,7 @@
         <v>403</v>
       </c>
       <c r="M137" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="138" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -7996,7 +7999,7 @@
         <v>406</v>
       </c>
       <c r="M138" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="139" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -8049,10 +8052,10 @@
         <v>410</v>
       </c>
       <c r="G140" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H140" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="I140" s="5" t="s">
         <v>346</v>
@@ -8079,10 +8082,10 @@
         <v>413</v>
       </c>
       <c r="G141" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H141" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="I141" s="5" t="s">
         <v>117</v>
@@ -8091,7 +8094,7 @@
         <v>414</v>
       </c>
       <c r="M141" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="142" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -8112,10 +8115,10 @@
         <v>413</v>
       </c>
       <c r="G142" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H142" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="I142" s="5" t="s">
         <v>117</v>
@@ -8176,7 +8179,7 @@
         <v>422</v>
       </c>
       <c r="G144" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H144" t="s">
         <v>689</v>
@@ -8243,7 +8246,7 @@
         <v>704</v>
       </c>
       <c r="H146" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I146" s="5" t="s">
         <v>113</v>
@@ -8272,7 +8275,7 @@
         <v>432</v>
       </c>
       <c r="G147" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="H147" t="s">
         <v>702</v>
@@ -8299,10 +8302,10 @@
         <v>435</v>
       </c>
       <c r="G148" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H148" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="I148" s="5" t="s">
         <v>43</v>
@@ -8393,10 +8396,10 @@
         <v>444</v>
       </c>
       <c r="G151" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H151" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I151" s="5" t="s">
         <v>151</v>
@@ -8487,10 +8490,10 @@
         <v>454</v>
       </c>
       <c r="G154" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H154" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="I154" s="5" t="s">
         <v>455</v>
@@ -8519,10 +8522,10 @@
         <v>459</v>
       </c>
       <c r="G155" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="H155" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I155" s="5" t="s">
         <v>309</v>
@@ -8583,7 +8586,7 @@
         <v>467</v>
       </c>
       <c r="G157" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H157" t="s">
         <v>694</v>
@@ -8615,7 +8618,7 @@
         <v>467</v>
       </c>
       <c r="G158" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H158" t="s">
         <v>694</v>
@@ -8679,10 +8682,10 @@
         <v>477</v>
       </c>
       <c r="G160" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="H160" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I160" s="5" t="s">
         <v>288</v>
@@ -8743,10 +8746,10 @@
         <v>485</v>
       </c>
       <c r="G162" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H162" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="I162" s="5" t="s">
         <v>288</v>
@@ -8775,7 +8778,7 @@
         <v>485</v>
       </c>
       <c r="G163" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H163" t="s">
         <v>679</v>
@@ -8807,10 +8810,10 @@
         <v>485</v>
       </c>
       <c r="G164" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H164" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="I164" s="5" t="s">
         <v>288</v>
@@ -8839,7 +8842,7 @@
         <v>485</v>
       </c>
       <c r="G165" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H165" t="s">
         <v>684</v>
@@ -8871,10 +8874,10 @@
         <v>485</v>
       </c>
       <c r="G166" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H166" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="I166" s="5" t="s">
         <v>288</v>
@@ -8903,7 +8906,7 @@
         <v>485</v>
       </c>
       <c r="G167" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H167" t="s">
         <v>684</v>
@@ -8935,10 +8938,10 @@
         <v>485</v>
       </c>
       <c r="G168" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H168" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="I168" s="5" t="s">
         <v>288</v>
@@ -8967,7 +8970,7 @@
         <v>485</v>
       </c>
       <c r="G169" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H169" t="s">
         <v>684</v>
@@ -8999,10 +9002,10 @@
         <v>485</v>
       </c>
       <c r="G170" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H170" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="I170" s="5" t="s">
         <v>288</v>
@@ -9031,7 +9034,7 @@
         <v>485</v>
       </c>
       <c r="G171" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H171" t="s">
         <v>684</v>
@@ -9239,10 +9242,10 @@
         <v>530</v>
       </c>
       <c r="G178" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="H178" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="I178" s="5" t="s">
         <v>11</v>
@@ -9269,10 +9272,10 @@
         <v>530</v>
       </c>
       <c r="G179" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="H179" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="I179" s="5" t="s">
         <v>11</v>
@@ -9455,7 +9458,7 @@
         <v>551</v>
       </c>
       <c r="G185" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H185" t="s">
         <v>689</v>
@@ -9470,7 +9473,7 @@
         <v>686</v>
       </c>
       <c r="M185" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="186" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -9491,10 +9494,10 @@
         <v>551</v>
       </c>
       <c r="G186" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="H186" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I186" s="5" t="s">
         <v>85</v>
@@ -9561,7 +9564,7 @@
         <v>694</v>
       </c>
       <c r="H188" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I188" s="5" t="s">
         <v>117</v>
@@ -9588,10 +9591,10 @@
         <v>561</v>
       </c>
       <c r="G189" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="H189" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I189" s="5" t="s">
         <v>151</v>
@@ -9620,10 +9623,10 @@
         <v>565</v>
       </c>
       <c r="G190" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H190" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="I190" s="5" t="s">
         <v>513</v>
@@ -9652,7 +9655,7 @@
         <v>565</v>
       </c>
       <c r="G191" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H191" t="s">
         <v>689</v>
@@ -9694,7 +9697,7 @@
         <v>573</v>
       </c>
       <c r="M192" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="193" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -9845,10 +9848,10 @@
         <v>590</v>
       </c>
       <c r="G197" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="H197" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="I197" s="5" t="s">
         <v>219</v>
@@ -9889,7 +9892,7 @@
         <v>595</v>
       </c>
       <c r="M198" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="199" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
@@ -9972,10 +9975,10 @@
         <v>604</v>
       </c>
       <c r="G201" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="H201" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="I201" s="5" t="s">
         <v>508</v>
@@ -9998,10 +10001,10 @@
         <v>607</v>
       </c>
       <c r="G202" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="H202" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="I202" s="5" t="s">
         <v>508</v>
@@ -10030,10 +10033,10 @@
         <v>610</v>
       </c>
       <c r="G203" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H203" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="I203" s="5" t="s">
         <v>513</v>
@@ -10060,10 +10063,10 @@
         <v>610</v>
       </c>
       <c r="G204" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="H204" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="I204" s="5" t="s">
         <v>513</v>
@@ -10224,7 +10227,7 @@
       </c>
       <c r="E222" s="3"/>
       <c r="H222" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.3">
@@ -10236,7 +10239,7 @@
       </c>
       <c r="E223" s="3"/>
       <c r="H223" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.3">
@@ -10387,7 +10390,7 @@
       </c>
       <c r="E241" s="3"/>
       <c r="H241" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>